<commit_message>
DRA example excel modified
</commit_message>
<xml_diff>
--- a/example/example-0001_dra_metadata.xlsx
+++ b/example/example-0001_dra_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\github\submission-excel2xml\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBBE3A3-C7CB-4129-B53C-B0A2DBB7066B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F22A8E5-400A-4951-8CFC-ADD5E5DE04B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1233,11 +1233,11 @@
     <t>Sentosa SQ301</t>
   </si>
   <si>
-    <t>2024-07-05 Bioinformation and DDBJ Center</t>
+    <t>2024-10-23 Bioinformation and DDBJ Center</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>v3.0</t>
+    <t>v3.1</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1712,7 +1712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
   <cols>

</xml_diff>